<commit_message>
adding changes of brunelle
</commit_message>
<xml_diff>
--- a/data/Ensegnement.xlsx
+++ b/data/Ensegnement.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fabio/Documents/Personal/MdC/Poste-ENSGSI/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4C7C896-7D0C-8D4F-B098-03E74FD94125}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75A4DC55-2A59-9743-BC96-9AFD2B95D9BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{EE5F1C4C-B231-1F43-9A5F-83FC6C4E0436}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="28300" xr2:uid="{EE5F1C4C-B231-1F43-9A5F-83FC6C4E0436}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Heures" sheetId="1" r:id="rId1"/>
+    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="74">
   <si>
     <r>
       <t>3</t>
@@ -94,9 +95,6 @@
     <t>BAC+5</t>
   </si>
   <si>
-    <t>POLE ENSGSI</t>
-  </si>
-  <si>
     <t>ENSGSI</t>
   </si>
   <si>
@@ -219,12 +217,138 @@
   <si>
     <t>2021 - 2022</t>
   </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>BAC+4</t>
+  </si>
+  <si>
+    <t>2017-2019</t>
+  </si>
+  <si>
+    <t>Conception et Innovation</t>
+  </si>
+  <si>
+    <t>Module Ingénierie de L'innovation II / Design Thinking</t>
+  </si>
+  <si>
+    <t>Introduction à la Recherche</t>
+  </si>
+  <si>
+    <t>Neuromarketing and Innovation</t>
+  </si>
+  <si>
+    <t>From Idea to Market</t>
+  </si>
+  <si>
+    <t>Introduction au prototypage et à l'Impression 3D</t>
+  </si>
+  <si>
+    <t>Formation Continue</t>
+  </si>
+  <si>
+    <t>BAC+1</t>
+  </si>
+  <si>
+    <t>Cursus préparatoire</t>
+  </si>
+  <si>
+    <t>Maths et Modélisation pour l'Ingénieur</t>
+  </si>
+  <si>
+    <t>Conception  Innovation</t>
+  </si>
+  <si>
+    <t>Génie des Matériaux</t>
+  </si>
+  <si>
+    <t>Génie méca./énergétique</t>
+  </si>
+  <si>
+    <t>Génie des Procédés</t>
+  </si>
+  <si>
+    <t>Ingénierie Système</t>
+  </si>
+  <si>
+    <t>Génie Industriel</t>
+  </si>
+  <si>
+    <t>Développement Durable Qualité</t>
+  </si>
+  <si>
+    <t>Gestion Entrepreneuriale</t>
+  </si>
+  <si>
+    <t>Management Projet Prof. et Perso.</t>
+  </si>
+  <si>
+    <t>Langues vivantes</t>
+  </si>
+  <si>
+    <t>Tutorat APS</t>
+  </si>
+  <si>
+    <t>Prépa</t>
+  </si>
+  <si>
+    <t>MMI</t>
+  </si>
+  <si>
+    <t>CI</t>
+  </si>
+  <si>
+    <t>GM</t>
+  </si>
+  <si>
+    <t>GME</t>
+  </si>
+  <si>
+    <t>GP</t>
+  </si>
+  <si>
+    <t>IS</t>
+  </si>
+  <si>
+    <t>GI</t>
+  </si>
+  <si>
+    <t>DDQ</t>
+  </si>
+  <si>
+    <t>GE</t>
+  </si>
+  <si>
+    <t>MP3</t>
+  </si>
+  <si>
+    <t>LV</t>
+  </si>
+  <si>
+    <t>APS</t>
+  </si>
+  <si>
+    <t>Animation et gestion d'un tiers-lieu dans son éco-système</t>
+  </si>
+  <si>
+    <t>Maîtrise des équipements et gestion éco-responsable des matériaux</t>
+  </si>
+  <si>
+    <t>Physique / Chimie</t>
+  </si>
+  <si>
+    <t>Pole</t>
+  </si>
+  <si>
+    <t>Prof. Coll. &amp; Lycée</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -271,6 +395,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -280,7 +426,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -357,18 +503,74 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
@@ -389,20 +591,11 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -416,6 +609,36 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -730,433 +953,725 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21CCC082-2532-3D44-BE97-A336697D3F90}">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="18.33203125" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" customWidth="1"/>
     <col min="3" max="4" width="14.33203125" customWidth="1"/>
     <col min="5" max="5" width="20.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="23.5" customWidth="1"/>
-    <col min="9" max="9" width="23.33203125" customWidth="1"/>
+    <col min="9" max="9" width="34.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="D2" s="15"/>
+      <c r="E2" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15">
+        <v>15</v>
+      </c>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15">
+        <v>4</v>
+      </c>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15">
+        <v>8</v>
+      </c>
+      <c r="H4" s="15"/>
+      <c r="I4" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15">
+        <v>16</v>
+      </c>
+      <c r="H5" s="15"/>
+      <c r="I5" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15">
+        <v>32</v>
+      </c>
+      <c r="H6" s="15"/>
+      <c r="I6" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="65" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="2">
+        <v>10.5</v>
+      </c>
+      <c r="G7" s="2">
+        <v>14.75</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="K7" s="12"/>
+    </row>
+    <row r="8" spans="1:11" ht="65" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4">
+        <v>15</v>
+      </c>
+      <c r="H8" s="4"/>
+      <c r="I8" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="K8" s="12"/>
+    </row>
+    <row r="9" spans="1:11" ht="49" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4">
+        <v>6.5</v>
+      </c>
+      <c r="H9" s="4"/>
+      <c r="I9" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="K9" s="12"/>
+    </row>
+    <row r="10" spans="1:11" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>25</v>
       </c>
-      <c r="F1" t="s">
+      <c r="B10" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2">
+        <v>3.75</v>
+      </c>
+      <c r="H10" s="2"/>
+      <c r="I10" s="22" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="49" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" s="4">
+        <v>2</v>
+      </c>
+      <c r="G11" s="4">
+        <v>4</v>
+      </c>
+      <c r="H11" s="4"/>
+      <c r="I11" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="49" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="65" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="9" t="s">
+      <c r="H12" s="4"/>
+      <c r="I12" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="49" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="2">
-        <v>10.5</v>
-      </c>
-      <c r="G2" s="2">
-        <v>14.75</v>
-      </c>
-      <c r="H2" s="2"/>
-      <c r="K2" s="15"/>
-    </row>
-    <row r="3" spans="1:11" ht="65" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4">
+      <c r="D13" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="4"/>
-      <c r="K3" s="15"/>
-    </row>
-    <row r="4" spans="1:11" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="5" t="s">
+      <c r="F13" s="4">
         <v>3</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4">
-        <v>6.5</v>
-      </c>
-      <c r="H4" s="4"/>
-      <c r="K4" s="15"/>
-    </row>
-    <row r="5" spans="1:11" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="10" t="s">
+      <c r="G13" s="4">
+        <v>6</v>
+      </c>
+      <c r="H13" s="4"/>
+      <c r="I13" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="41" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2">
-        <v>3.75</v>
-      </c>
-      <c r="H5" s="2"/>
-    </row>
-    <row r="6" spans="1:11" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="F6" s="4">
-        <v>2</v>
-      </c>
-      <c r="G6" s="4">
-        <v>4</v>
-      </c>
-      <c r="H6" s="4"/>
-    </row>
-    <row r="7" spans="1:11" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4">
-        <v>6</v>
-      </c>
-      <c r="H7" s="4"/>
-    </row>
-    <row r="8" spans="1:11" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="4">
-        <v>3</v>
-      </c>
-      <c r="G8" s="4">
-        <v>6</v>
-      </c>
-      <c r="H8" s="4"/>
-    </row>
-    <row r="9" spans="1:11" ht="41" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="12" t="s">
+      <c r="D14" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="7" t="s">
+      <c r="E14" s="6" t="s">
         <v>18</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="4">
-        <v>3</v>
-      </c>
-      <c r="G9" s="4">
-        <v>12</v>
-      </c>
-      <c r="H9" s="4">
-        <v>9</v>
-      </c>
-      <c r="K9" s="14"/>
-    </row>
-    <row r="10" spans="1:11" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" s="4">
-        <v>2</v>
-      </c>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4">
-        <v>5.5</v>
-      </c>
-      <c r="K10" s="14"/>
-    </row>
-    <row r="11" spans="1:11" ht="33" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4">
-        <v>2</v>
-      </c>
-      <c r="H11" s="4">
-        <v>1</v>
-      </c>
-      <c r="K11" s="15"/>
-    </row>
-    <row r="12" spans="1:11" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2">
-        <v>12</v>
-      </c>
-      <c r="K12" s="15"/>
-    </row>
-    <row r="13" spans="1:11" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4">
-        <v>20</v>
-      </c>
-      <c r="H13" s="4"/>
-      <c r="K13" s="15"/>
-    </row>
-    <row r="14" spans="1:11" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>1</v>
       </c>
       <c r="F14" s="4">
         <v>3</v>
       </c>
       <c r="G14" s="4">
-        <v>4.5</v>
-      </c>
-      <c r="H14" s="4"/>
-      <c r="K14" s="15"/>
-    </row>
-    <row r="15" spans="1:11" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" s="4">
+        <v>9</v>
+      </c>
+      <c r="I14" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="K14" s="11"/>
+    </row>
+    <row r="15" spans="1:11" ht="65" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="4">
+        <v>2</v>
+      </c>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4">
+        <v>5.5</v>
+      </c>
+      <c r="I15" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="K15" s="11"/>
+    </row>
+    <row r="16" spans="1:11" ht="65" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4">
+        <v>2</v>
+      </c>
+      <c r="H16" s="4">
+        <v>1</v>
+      </c>
+      <c r="I16" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="K16" s="12"/>
+    </row>
+    <row r="17" spans="1:11" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="E15" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15" s="4">
-        <v>3.5</v>
-      </c>
-      <c r="G15" s="4">
-        <v>4</v>
-      </c>
-      <c r="H15" s="4"/>
-      <c r="K15" s="15"/>
-    </row>
-    <row r="16" spans="1:11" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F16" s="4">
-        <v>6</v>
-      </c>
-      <c r="G16" s="4">
-        <v>6</v>
-      </c>
-      <c r="H16" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17" s="11"/>
-      <c r="E17" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F17" s="4">
-        <v>6</v>
-      </c>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="33" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D18" s="8"/>
+      <c r="B17" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2">
+        <v>12</v>
+      </c>
+      <c r="I17" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="K17" s="12"/>
+    </row>
+    <row r="18" spans="1:11" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="E18" s="6" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="F18" s="4"/>
       <c r="G18" s="4">
+        <v>20</v>
+      </c>
+      <c r="H18" s="4"/>
+      <c r="I18" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="K18" s="12"/>
+    </row>
+    <row r="19" spans="1:11" ht="49" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F19" s="4">
         <v>3</v>
       </c>
-      <c r="H18" s="4">
+      <c r="G19" s="4">
+        <v>4.5</v>
+      </c>
+      <c r="H19" s="4"/>
+      <c r="I19" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="K19" s="12"/>
+    </row>
+    <row r="20" spans="1:11" ht="49" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" s="4">
+        <v>3.5</v>
+      </c>
+      <c r="G20" s="4">
+        <v>4</v>
+      </c>
+      <c r="H20" s="4"/>
+      <c r="I20" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="K20" s="12"/>
+    </row>
+    <row r="21" spans="1:11" ht="49" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" s="4">
+        <v>6</v>
+      </c>
+      <c r="G21" s="4">
+        <v>6</v>
+      </c>
+      <c r="H21" s="4">
+        <v>12</v>
+      </c>
+      <c r="I21" s="23" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="65" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F22" s="4">
+        <v>6</v>
+      </c>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4">
+        <v>9</v>
+      </c>
+      <c r="I22" s="15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="65" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4">
         <v>3</v>
       </c>
+      <c r="H23" s="4">
+        <v>3</v>
+      </c>
+      <c r="I23" s="15" t="s">
+        <v>69</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="D16:D18"/>
-    <mergeCell ref="D9:D11"/>
-  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0530B033-1876-0743-BF48-5B5219BDEC3A}">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:13" ht="56" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="L1" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="M1" s="18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="I2" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="J2" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="K2" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="L2" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="M2" s="21" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>